<commit_message>
Updated the pinout with uSD and DCMI interfaces
</commit_message>
<xml_diff>
--- a/pinOut.xlsx
+++ b/pinOut.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="140">
   <si>
     <t>PA0</t>
   </si>
@@ -391,6 +391,54 @@
   </si>
   <si>
     <t>TxD1</t>
+  </si>
+  <si>
+    <t>MDC</t>
+  </si>
+  <si>
+    <t>uSD</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>CMD</t>
+  </si>
+  <si>
+    <t>HSYNC</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
+    <t>PIXCK</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>VSYNC</t>
   </si>
 </sst>
 </file>
@@ -733,7 +781,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +802,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -781,24 +829,36 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,142 +872,184 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>127</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>126</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -974,347 +1076,419 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -1330,7 +1504,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -1357,7 +1531,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Just added the uSD card to the schematic and connected it to the processor
</commit_message>
<xml_diff>
--- a/pinOut.xlsx
+++ b/pinOut.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="142">
   <si>
     <t>PA0</t>
   </si>
@@ -439,6 +439,12 @@
   </si>
   <si>
     <t>VSYNC</t>
+  </si>
+  <si>
+    <t>NOTES:</t>
+  </si>
+  <si>
+    <t>not needed for uSD</t>
   </si>
 </sst>
 </file>
@@ -777,11 +783,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23:C23"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +797,7 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -801,13 +807,16 @@
       <c r="C1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -818,7 +827,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -829,12 +838,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -845,12 +854,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -861,7 +870,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -872,12 +881,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -888,7 +897,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -899,62 +908,62 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -965,7 +974,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -976,7 +985,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -986,8 +995,11 @@
       <c r="C26" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -997,43 +1009,46 @@
       <c r="C27" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1044,17 +1059,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1065,7 +1080,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1076,7 +1091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1086,8 +1101,11 @@
       <c r="C40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1097,8 +1115,11 @@
       <c r="C41" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1109,50 +1130,56 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C43" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>

</xml_diff>

<commit_message>
Removed the un-needed pins that I had allocated for SDIO
</commit_message>
<xml_diff>
--- a/pinOut.xlsx
+++ b/pinOut.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
   <si>
     <t>PA0</t>
   </si>
@@ -442,9 +442,6 @@
   </si>
   <si>
     <t>NOTES:</t>
-  </si>
-  <si>
-    <t>not needed for uSD</t>
   </si>
 </sst>
 </file>
@@ -783,11 +780,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,12 +809,12 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -827,7 +825,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -838,12 +836,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -854,12 +852,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -870,7 +868,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -881,12 +879,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -897,7 +895,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -908,62 +906,62 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -974,7 +972,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -985,70 +983,52 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" t="s">
-        <v>125</v>
-      </c>
-      <c r="D26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" t="s">
-        <v>125</v>
-      </c>
-      <c r="D27" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1059,17 +1039,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1080,7 +1060,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1091,35 +1071,17 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" t="s">
-        <v>125</v>
-      </c>
-      <c r="D40" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>129</v>
-      </c>
-      <c r="C41" t="s">
-        <v>125</v>
-      </c>
-      <c r="D41" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1130,7 +1092,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1141,7 +1103,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1152,7 +1114,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1163,7 +1125,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1174,27 +1136,27 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1210,72 +1172,72 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1286,7 +1248,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1297,17 +1259,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1318,7 +1280,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1329,7 +1291,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1340,187 +1302,187 @@
         <v>136</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -1531,12 +1493,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -1547,7 +1509,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -1558,13 +1520,19 @@
         <v>116</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C113"/>
+  <autoFilter ref="A1:C113">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="uSD"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated the Pin Out.xlsx
Adding the STM32F4 Discovery datasheet

Finished the header layout from the discovery
</commit_message>
<xml_diff>
--- a/pinOut.xlsx
+++ b/pinOut.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="186">
   <si>
     <t>PA0</t>
   </si>
@@ -442,6 +442,141 @@
   </si>
   <si>
     <t>NOTES:</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>PowerOn</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>VBUS</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>SWDIO</t>
+  </si>
+  <si>
+    <t>SWD</t>
+  </si>
+  <si>
+    <t>SWCLK</t>
+  </si>
+  <si>
+    <t>SWO</t>
+  </si>
+  <si>
+    <t>DevBoard</t>
+  </si>
+  <si>
+    <t>SCL/SPC</t>
+  </si>
+  <si>
+    <t>Accel</t>
+  </si>
+  <si>
+    <t>SDO</t>
+  </si>
+  <si>
+    <t>SDA/SDI/SDO</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>BlueButton</t>
+  </si>
+  <si>
+    <t>LRCK/AIN1x</t>
+  </si>
+  <si>
+    <t>DAC/Audio</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>CLK</t>
+  </si>
+  <si>
+    <t>Mic</t>
+  </si>
+  <si>
+    <t>DOUT/AIN4x</t>
+  </si>
+  <si>
+    <t>MCLK</t>
+  </si>
+  <si>
+    <t>SCLK</t>
+  </si>
+  <si>
+    <t>SDIN</t>
+  </si>
+  <si>
+    <t>OSC32_IN</t>
+  </si>
+  <si>
+    <t>OSC</t>
+  </si>
+  <si>
+    <t>OSC32_OUT</t>
+  </si>
+  <si>
+    <t>RESET</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>OverCurrent</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>INT1</t>
+  </si>
+  <si>
+    <t>INT2</t>
+  </si>
+  <si>
+    <t>CS_I2C/SPI</t>
+  </si>
+  <si>
+    <t>PH0</t>
+  </si>
+  <si>
+    <t>PH1</t>
+  </si>
+  <si>
+    <t>OSC_IN</t>
+  </si>
+  <si>
+    <t>OSC_OUT</t>
   </si>
 </sst>
 </file>
@@ -780,21 +915,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42:C46"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>112</v>
       </c>
@@ -805,15 +942,27 @@
         <v>114</v>
       </c>
       <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -824,7 +973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -835,12 +984,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -850,13 +999,25 @@
       <c r="C6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>152</v>
+      </c>
+      <c r="E7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -866,8 +1027,11 @@
       <c r="C8" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -877,90 +1041,168 @@
       <c r="C9" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="D12" t="s">
+        <v>146</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+      <c r="D13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E21" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -970,8 +1212,14 @@
       <c r="C24" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -982,52 +1230,94 @@
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>123</v>
+      </c>
+      <c r="C31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s">
+        <v>141</v>
+      </c>
+      <c r="D34" t="s">
+        <v>142</v>
+      </c>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1038,17 +1328,23 @@
         <v>116</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>166</v>
+      </c>
+      <c r="E37" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1059,7 +1355,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1070,17 +1366,35 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
+      </c>
+      <c r="D41" t="s">
+        <v>167</v>
+      </c>
+      <c r="E41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1091,7 +1405,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1102,7 +1416,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1112,8 +1426,14 @@
       <c r="C44" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>168</v>
+      </c>
+      <c r="E44" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1124,7 +1444,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1134,33 +1454,51 @@
       <c r="C46" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" t="s">
+        <v>172</v>
+      </c>
+      <c r="E49" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1171,72 +1509,114 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" t="s">
+        <v>141</v>
+      </c>
+      <c r="D55" t="s">
+        <v>174</v>
+      </c>
+      <c r="E55" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>176</v>
+      </c>
+      <c r="E62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
+        <v>178</v>
+      </c>
+      <c r="E65" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1246,8 +1626,14 @@
       <c r="C66" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>179</v>
+      </c>
+      <c r="E66" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1257,18 +1643,30 @@
       <c r="C67" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>180</v>
+      </c>
+      <c r="E67" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>181</v>
+      </c>
+      <c r="E68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1279,7 +1677,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1290,7 +1688,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1301,42 +1699,42 @@
         <v>136</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1346,182 +1744,186 @@
         <v>79</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109" t="s">
-        <v>121</v>
-      </c>
-      <c r="C109" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>109</v>
       </c>
-      <c r="B111" t="s">
-        <v>122</v>
-      </c>
-      <c r="C111" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B112" t="s">
-        <v>123</v>
-      </c>
-      <c r="C112" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>182</v>
+      </c>
+      <c r="D114" t="s">
+        <v>184</v>
+      </c>
+      <c r="E114" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>183</v>
+      </c>
+      <c r="D115" t="s">
+        <v>185</v>
+      </c>
+      <c r="E115" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pushing the pinOut without a filter applied
</commit_message>
<xml_diff>
--- a/pinOut.xlsx
+++ b/pinOut.xlsx
@@ -672,13 +672,13 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:F115"/>
@@ -688,11 +688,12 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.03137254901961"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4745098039216"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9058823529412"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.06666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.956862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5254901960784"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.54117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
@@ -715,7 +716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
@@ -726,7 +727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>8</v>
       </c>
@@ -737,7 +738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>11</v>
       </c>
@@ -748,7 +749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
@@ -770,7 +771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
@@ -795,7 +796,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>25</v>
       </c>
@@ -812,12 +813,12 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>29</v>
       </c>
@@ -834,7 +835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>34</v>
       </c>
@@ -851,7 +852,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
         <v>36</v>
       </c>
@@ -868,7 +869,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
         <v>38</v>
       </c>
@@ -885,7 +886,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>40</v>
       </c>
@@ -902,7 +903,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>43</v>
       </c>
@@ -919,27 +920,27 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
         <v>45</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>48</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>49</v>
       </c>
@@ -956,12 +957,12 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>51</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
         <v>52</v>
       </c>
@@ -994,12 +995,12 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>58</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>59</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>61</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>64</v>
       </c>
@@ -1032,7 +1033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>66</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>68</v>
       </c>
@@ -1054,17 +1055,17 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>70</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>72</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>31</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>74</v>
       </c>
@@ -1092,12 +1093,12 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>76</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>77</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>63</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>79</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>81</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="42">
       <c r="A42" s="2" t="s">
         <v>88</v>
       </c>
@@ -1171,7 +1172,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="43">
       <c r="A43" s="2" t="s">
         <v>90</v>
       </c>
@@ -1184,7 +1185,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="44">
       <c r="A44" s="2" t="s">
         <v>91</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="45">
       <c r="A45" s="2" t="s">
         <v>94</v>
       </c>
@@ -1214,7 +1215,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="46">
       <c r="A46" s="2" t="s">
         <v>96</v>
       </c>
@@ -1231,12 +1232,12 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>99</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>100</v>
       </c>
@@ -1247,7 +1248,7 @@
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>103</v>
       </c>
@@ -1258,17 +1259,17 @@
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
         <v>105</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
         <v>106</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="52">
       <c r="A52" s="2" t="s">
         <v>107</v>
       </c>
@@ -1281,12 +1282,12 @@
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
         <v>109</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
         <v>110</v>
       </c>
@@ -1297,7 +1298,7 @@
         <v>18</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>112</v>
       </c>
@@ -1314,37 +1315,37 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="56">
       <c r="A56" s="0" t="s">
         <v>115</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="57">
       <c r="A57" s="0" t="s">
         <v>116</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>117</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="59">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="59">
       <c r="A59" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="60">
       <c r="A60" s="0" t="s">
         <v>119</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="61">
       <c r="A61" s="0" t="s">
         <v>120</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="62">
       <c r="A62" s="0" t="s">
         <v>121</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="63">
       <c r="A63" s="0" t="s">
         <v>123</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="64">
       <c r="A64" s="0" t="s">
         <v>125</v>
       </c>
@@ -1377,7 +1378,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="65">
       <c r="A65" s="0" t="s">
         <v>126</v>
       </c>
@@ -1422,7 +1423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="68">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
         <v>132</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="69">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
         <v>134</v>
       </c>
@@ -1471,47 +1472,47 @@
         <v>16</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="73">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
         <v>141</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="74">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
         <v>142</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="75">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
         <v>143</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>144</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="77">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
         <v>145</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="78">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
         <v>146</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>147</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>148</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.75" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>149</v>
       </c>
@@ -1676,7 +1677,7 @@
         <v>181</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="114">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="114">
       <c r="A114" s="0" t="s">
         <v>182</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>102</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="true" ht="12.75" outlineLevel="0" r="115">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="115">
       <c r="A115" s="0" t="s">
         <v>184</v>
       </c>
@@ -1699,13 +1700,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C113">
-    <filterColumn colId="2">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Camera"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C113"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
@@ -1728,6 +1723,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1750,6 +1748,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.54117647058824"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>